<commit_message>
add HTML mail body
</commit_message>
<xml_diff>
--- a/linkedin_data.xlsx
+++ b/linkedin_data.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -930,6 +930,78 @@
         <v>2</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>gamodemy1@gmail.com</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>20-June, 22:55</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>gamodemy1@gmail.com</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>20-June, 23:04</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>4</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>gamodemy1@gmail.com</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>20-June, 23:07</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>4</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>